<commit_message>
Updated data import setup matrix to add All Utilities dimension to several inputs. Have not yet added that dimensionality to the actual model data nodes though.
</commit_message>
<xml_diff>
--- a/TTD2.xlsx
+++ b/TTD2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwelch\Documents\Repos\Nexant\SPIDER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49AD594-6EA7-46E4-9CF8-733B0C9942E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190247B2-2AD5-4D17-84DB-621D76916135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5146E2CE-1DA6-49DB-8CCB-E1EDEC8E22DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5146E2CE-1DA6-49DB-8CCB-E1EDEC8E22DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Task</t>
   </si>
@@ -177,6 +177,12 @@
   </si>
   <si>
     <t>Make Area Type a user defined categorical index</t>
+  </si>
+  <si>
+    <t>Fix incentive input format and import from data template</t>
+  </si>
+  <si>
+    <t>Make historical PV/storage adoption new tabs in data template</t>
   </si>
 </sst>
 </file>
@@ -590,7 +596,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43FCDD1C-2E4F-4EFA-B56C-BABF1F902BD3}">
-  <dimension ref="C1:P11"/>
+  <dimension ref="C1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
@@ -737,6 +743,16 @@
         <v>24</v>
       </c>
     </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>